<commit_message>
updates for generating CSDCO dta packages
</commit_message>
<xml_diff>
--- a/CSDCODirWalkTests/godirwalk/output/report.xlsx
+++ b/CSDCODirWalkTests/godirwalk/output/report.xlsx
@@ -602,7 +602,7 @@
         <v>GLAD7 (Malawi)</v>
       </c>
       <c r="B1" s="1" t="str">
-        <v>/sample requests/SRF_GLAD7_Johnson_20081201/LacCore_SRF_part2of2_GLAD7_Johnson_20081201.xls</v>
+        <v>/sample requests/SRF_GLAD7_Johnson_20081201/~$hnson_SRF_part1of2.doc</v>
       </c>
       <c r="C1" s="1" t="str"/>
       <c r="D1" s="1" t="str">
@@ -614,7 +614,7 @@
         <v>GLAD7 (Malawi)</v>
       </c>
       <c r="B2" s="2" t="str">
-        <v>/sample requests/MAL05-TCJ-sampls.xls</v>
+        <v>/sample requests/GLAD7JohnsonTEX86.xls</v>
       </c>
       <c r="C2" s="2" t="str"/>
       <c r="D2" s="2" t="str">
@@ -626,7 +626,7 @@
         <v>GLAD7 (Malawi)</v>
       </c>
       <c r="B3" s="3" t="str">
-        <v>/sample requests/GLAD7 sampling_20070109.xls</v>
+        <v>/sample requests/SRF2_GLAD7_Scholz_20070112.xls</v>
       </c>
       <c r="C3" s="3" t="str"/>
       <c r="D3" s="3" t="str">
@@ -634,15 +634,17 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B4" s="4" t="str">
-        <v>/sample requests/LacCore_SRF_part2of2_Abbott_20090917.xls</v>
-      </c>
-      <c r="C4" s="4" t="str"/>
-      <c r="D4" s="4" t="str">
-        <v>notvalid</v>
+      <c r="A4" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B4" t="str">
+        <v>/sample requests/SRF_GLAD7_Johnson_20081201/images/GLAD7-MAL05-1B-45E-2 copy.bmp</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Images</v>
+      </c>
+      <c r="D4" t="str">
+        <v>valid</v>
       </c>
     </row>
     <row r="5">
@@ -650,7 +652,7 @@
         <v>GLAD7 (Malawi)</v>
       </c>
       <c r="B5" t="str">
-        <v>/sample requests/SRF_GLAD7_Johnson_20081201/images/GLAD7-MAL05-1B-42E-3 copy.bmp</v>
+        <v>/sample requests/SRF_GLAD7_Johnson_20081201/images/GLAD7-MAL05-1B-43E-2 copy.bmp</v>
       </c>
       <c r="C5" t="str">
         <v>Images</v>
@@ -660,176 +662,176 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B6" t="str">
+      <c r="A6" s="4" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B6" s="4" t="str">
+        <v>/sample requests/SRF_GLAD7_Johnson_20081201/Johnson_SRF_part2of2.doc</v>
+      </c>
+      <c r="C6" s="4" t="str"/>
+      <c r="D6" s="4" t="str">
+        <v>notvalid</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B7" t="str">
+        <v>GLAD7-metadata.xls</v>
+      </c>
+      <c r="C7" t="str">
+        <v>metadata</v>
+      </c>
+      <c r="D7" t="str">
+        <v>valid</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B8" t="str">
         <v>/sample requests/SRF_GLAD7_Johnson_20081201/images/GLAD7-MAL05-1B-44E-4 copy.bmp</v>
       </c>
-      <c r="C6" t="str">
+      <c r="C8" t="str">
         <v>Images</v>
       </c>
-      <c r="D6" t="str">
+      <c r="D8" t="str">
         <v>valid</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="5" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B7" s="5" t="str">
-        <v>/sample requests/SRF_GLAD7_Johnson_20081201/Johnson_SRF_part2of2.doc</v>
-      </c>
-      <c r="C7" s="5" t="str"/>
-      <c r="D7" s="5" t="str">
-        <v>notvalid</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="6" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B8" s="6" t="str">
+    <row r="9">
+      <c r="A9" s="5" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B9" s="5" t="str">
+        <v>/sample requests/GLAD7_Petrick_C14_20090302/LacCore_GLAD7_SRF_part1of2.doc</v>
+      </c>
+      <c r="C9" s="5" t="str"/>
+      <c r="D9" s="5" t="str">
+        <v>notvalid</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B10" t="str">
+        <v>/sample requests/SRF_GLAD7_Johnson_20081201/images/GLAD7-MAL05-1B-42E-3 copy.bmp</v>
+      </c>
+      <c r="C10" t="str">
+        <v>Images</v>
+      </c>
+      <c r="D10" t="str">
+        <v>valid</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="6" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B11" s="6" t="str">
+        <v>/sample requests/LacCore_SRF_part2of2_Abbott_20090917.xls</v>
+      </c>
+      <c r="C11" s="6" t="str"/>
+      <c r="D11" s="6" t="str">
+        <v>notvalid</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="7" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B12" s="7" t="str">
+        <v>/sample requests/MAL05-TCJ-sampls.xls</v>
+      </c>
+      <c r="C12" s="7" t="str"/>
+      <c r="D12" s="7" t="str">
+        <v>notvalid</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B13" s="8" t="str">
+        <v>/sample requests/GLAD7_Stone_diatoms_20061026/GLAD7_Stone_diatoms_20061026.xls</v>
+      </c>
+      <c r="C13" s="8" t="str"/>
+      <c r="D13" s="8" t="str">
+        <v>notvalid</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="9" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B14" s="9" t="str">
+        <v>/sample requests/MALsamples4_15to4_17.xlsx</v>
+      </c>
+      <c r="C14" s="9" t="str"/>
+      <c r="D14" s="9" t="str">
+        <v>notvalid</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B15" s="10" t="str">
+        <v>/sample requests/SRF_GLAD7_Johnson_20081201/LacCore_SRF_part2of2_GLAD7_Johnson_20081201.xls</v>
+      </c>
+      <c r="C15" s="10" t="str"/>
+      <c r="D15" s="10" t="str">
+        <v>notvalid</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="11" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B16" s="11" t="str">
+        <v>/sample requests/GLAD7_Beuning_pollen_20061103/LacCore_SRF_part2of2 Nov 2006.xls</v>
+      </c>
+      <c r="C16" s="11" t="str"/>
+      <c r="D16" s="11" t="str">
+        <v>notvalid</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="12" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B17" s="12" t="str">
+        <v>/sample requests/MW LacCore_SRF_part2of2.xls</v>
+      </c>
+      <c r="C17" s="12" t="str"/>
+      <c r="D17" s="12" t="str">
+        <v>notvalid</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="13" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B18" s="13" t="str">
         <v>/sample requests/GLAD7_Petrick_C14_20090302/LacCore_GLAD7_SRF_part2of2 ETB.xls</v>
       </c>
-      <c r="C8" s="6" t="str"/>
-      <c r="D8" s="6" t="str">
-        <v>notvalid</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B9" s="7" t="str">
-        <v>/sample requests/SRF2_GLAD7_Scholz_20070112.xls</v>
-      </c>
-      <c r="C9" s="7" t="str"/>
-      <c r="D9" s="7" t="str">
-        <v>notvalid</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="8" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B10" s="8" t="str">
-        <v>/sample requests/GLAD7_Beuning_pollen_20061103/LacCore_SRF_part2of2 Nov 2006.xls</v>
-      </c>
-      <c r="C10" s="8" t="str"/>
-      <c r="D10" s="8" t="str">
-        <v>notvalid</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B11" t="str">
-        <v>GLAD7-metadata.xls</v>
-      </c>
-      <c r="C11" t="str">
-        <v>metadata</v>
-      </c>
-      <c r="D11" t="str">
-        <v>valid</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="9" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B12" s="9" t="str">
-        <v>/sample requests/MW LacCore_SRF_part2of2.xls</v>
-      </c>
-      <c r="C12" s="9" t="str"/>
-      <c r="D12" s="9" t="str">
-        <v>notvalid</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="10" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B13" s="10" t="str">
-        <v>/sample requests/LacCore_SRF_part2of2complete_Ivory.xls</v>
-      </c>
-      <c r="C13" s="10" t="str"/>
-      <c r="D13" s="10" t="str">
-        <v>notvalid</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="11" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B14" s="11" t="str">
-        <v>/sample requests/SRF_GLAD7_Johnson_20081201/ptf-Johnson_GLAD7_20081201.doc</v>
-      </c>
-      <c r="C14" s="11" t="str"/>
-      <c r="D14" s="11" t="str">
-        <v>notvalid</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B15" t="str">
-        <v>/sample requests/SRF_GLAD7_Johnson_20081201/images/GLAD7-MAL05-1B-42E-2 copy.bmp</v>
-      </c>
-      <c r="C15" t="str">
-        <v>Images</v>
-      </c>
-      <c r="D15" t="str">
-        <v>valid</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="12" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B16" s="12" t="str">
-        <v>/sample requests/GLAD7JohnsonTEX86.xls</v>
-      </c>
-      <c r="C16" s="12" t="str"/>
-      <c r="D16" s="12" t="str">
-        <v>notvalid</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="13" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B17" s="13" t="str">
+      <c r="C18" s="13" t="str"/>
+      <c r="D18" s="13" t="str">
+        <v>notvalid</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="14" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B19" s="14" t="str">
         <v>/sample requests/SRF_GLAD7_Johnson_20081201/Johnson_SRF_part1of2.doc</v>
       </c>
-      <c r="C17" s="13" t="str"/>
-      <c r="D17" s="13" t="str">
-        <v>notvalid</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="14" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B18" s="14" t="str">
-        <v>/sample requests/MALsamples4_15to4_17.xlsx</v>
-      </c>
-      <c r="C18" s="14" t="str"/>
-      <c r="D18" s="14" t="str">
-        <v>notvalid</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="15" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B19" s="15" t="str">
-        <v>/sample requests/SRF_GLAD7_Johnson_20081201/~$hnson_SRF_part1of2.doc</v>
-      </c>
-      <c r="C19" s="15" t="str"/>
-      <c r="D19" s="15" t="str">
+      <c r="C19" s="14" t="str"/>
+      <c r="D19" s="14" t="str">
         <v>notvalid</v>
       </c>
     </row>
@@ -838,7 +840,7 @@
         <v>GLAD7 (Malawi)</v>
       </c>
       <c r="B20" t="str">
-        <v>/sample requests/SRF_GLAD7_Johnson_20081201/images/GLAD7-MAL05-1B-45E-2 copy.bmp</v>
+        <v>/sample requests/SRF_GLAD7_Johnson_20081201/images/GLAD7-MAL05-1B-42E-2 copy.bmp</v>
       </c>
       <c r="C20" t="str">
         <v>Images</v>
@@ -848,41 +850,39 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="16" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B21" s="16" t="str">
-        <v>/sample requests/GLAD7_Stone_diatoms_20061026/GLAD7_Stone_diatoms_20061026.xls</v>
-      </c>
-      <c r="C21" s="16" t="str"/>
-      <c r="D21" s="16" t="str">
+      <c r="A21" s="15" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B21" s="15" t="str">
+        <v>/sample requests/GLAD7 sampling_20070109.xls</v>
+      </c>
+      <c r="C21" s="15" t="str"/>
+      <c r="D21" s="15" t="str">
         <v>notvalid</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="17" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B22" s="17" t="str">
-        <v>/sample requests/GLAD7_Petrick_C14_20090302/LacCore_GLAD7_SRF_part1of2.doc</v>
-      </c>
-      <c r="C22" s="17" t="str"/>
-      <c r="D22" s="17" t="str">
+      <c r="A22" s="16" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B22" s="16" t="str">
+        <v>/sample requests/LacCore_SRF_part2of2complete_Ivory.xls</v>
+      </c>
+      <c r="C22" s="16" t="str"/>
+      <c r="D22" s="16" t="str">
         <v>notvalid</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="str">
-        <v>GLAD7 (Malawi)</v>
-      </c>
-      <c r="B23" t="str">
-        <v>/sample requests/SRF_GLAD7_Johnson_20081201/images/GLAD7-MAL05-1B-43E-2 copy.bmp</v>
-      </c>
-      <c r="C23" t="str">
-        <v>Images</v>
-      </c>
-      <c r="D23" t="str">
-        <v>valid</v>
+      <c r="A23" s="17" t="str">
+        <v>GLAD7 (Malawi)</v>
+      </c>
+      <c r="B23" s="17" t="str">
+        <v>/sample requests/SRF_GLAD7_Johnson_20081201/ptf-Johnson_GLAD7_20081201.doc</v>
+      </c>
+      <c r="C23" s="17" t="str"/>
+      <c r="D23" s="17" t="str">
+        <v>notvalid</v>
       </c>
     </row>
   </sheetData>

</xml_diff>